<commit_message>
depuracion de codigo y desarrollo de sidebar
</commit_message>
<xml_diff>
--- a/Aplicacion Final/2024/Resumen_Partidos_AL_2024.xlsx
+++ b/Aplicacion Final/2024/Resumen_Partidos_AL_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\Aplicacion Final\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA667E4-CECF-48AC-B288-74D8053AD3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C2237A-C34C-4C1C-B4DF-8407D5777421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen_Partidos_AL_2024" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>id_jornada</t>
   </si>
@@ -338,6 +338,27 @@
   </si>
   <si>
     <t>Enderson Moreira</t>
+  </si>
+  <si>
+    <t>Posicion resultante</t>
+  </si>
+  <si>
+    <t>Importancia</t>
+  </si>
+  <si>
+    <t>Puntos1</t>
+  </si>
+  <si>
+    <t>Puntos2</t>
+  </si>
+  <si>
+    <t>PuntosDif1</t>
+  </si>
+  <si>
+    <t>PuntosDif2</t>
+  </si>
+  <si>
+    <t>Puntos jugados</t>
   </si>
 </sst>
 </file>
@@ -700,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,9 +741,14 @@
     <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +785,29 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -797,8 +844,29 @@
       <c r="L2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -835,8 +903,29 @@
       <c r="L3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -873,8 +962,29 @@
       <c r="L4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <v>9</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -911,8 +1021,29 @@
       <c r="L5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>12</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -949,8 +1080,29 @@
       <c r="L6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>13</v>
+      </c>
+      <c r="P6">
+        <v>13</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -987,8 +1139,29 @@
       <c r="L7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>16</v>
+      </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1025,8 +1198,29 @@
       <c r="L8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>19</v>
+      </c>
+      <c r="P8">
+        <v>17</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1063,8 +1257,29 @@
       <c r="L9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <v>19</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1101,8 +1316,29 @@
       <c r="L10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>22</v>
+      </c>
+      <c r="P10">
+        <v>21</v>
+      </c>
+      <c r="Q10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1139,8 +1375,29 @@
       <c r="L11">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>25</v>
+      </c>
+      <c r="P11">
+        <v>24</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1177,8 +1434,29 @@
       <c r="L12">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>28</v>
+      </c>
+      <c r="P12">
+        <v>27</v>
+      </c>
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <v>6</v>
+      </c>
+      <c r="S12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1215,8 +1493,29 @@
       <c r="L13">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>30</v>
+      </c>
+      <c r="Q13">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>6</v>
+      </c>
+      <c r="S13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1253,8 +1552,29 @@
       <c r="L14">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>33</v>
+      </c>
+      <c r="P14">
+        <v>31</v>
+      </c>
+      <c r="Q14">
+        <v>9</v>
+      </c>
+      <c r="R14">
+        <v>7</v>
+      </c>
+      <c r="S14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1291,8 +1611,29 @@
       <c r="L15">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>34</v>
+      </c>
+      <c r="P15">
+        <v>33</v>
+      </c>
+      <c r="Q15">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>6</v>
+      </c>
+      <c r="S15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1329,8 +1670,29 @@
       <c r="L16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>36</v>
+      </c>
+      <c r="P16">
+        <v>34</v>
+      </c>
+      <c r="Q16">
+        <v>6</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1367,8 +1729,29 @@
       <c r="L17">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>37</v>
+      </c>
+      <c r="P17">
+        <v>37</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -1405,8 +1788,29 @@
       <c r="L18">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>40</v>
+      </c>
+      <c r="P18">
+        <v>40</v>
+      </c>
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>7</v>
+      </c>
+      <c r="S18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1443,8 +1847,29 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1481,8 +1906,29 @@
       <c r="L20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -1519,8 +1965,29 @@
       <c r="L21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>2</v>
+      </c>
+      <c r="S21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1557,8 +2024,29 @@
       <c r="L22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>5</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1595,8 +2083,29 @@
       <c r="L23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>11</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>4</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1632,6 +2141,27 @@
       </c>
       <c r="L24">
         <v>4</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>5</v>
+      </c>
+      <c r="O24">
+        <v>14</v>
+      </c>
+      <c r="P24">
+        <v>6</v>
+      </c>
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>